<commit_message>
parser and status display
</commit_message>
<xml_diff>
--- a/documents/Codes.xlsx
+++ b/documents/Codes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\EV inverter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\EV bms\bms\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -857,12 +857,12 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="87.42578125" customWidth="1"/>
+    <col min="1" max="1" width="98.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="5.5703125" customWidth="1"/>
@@ -987,6 +987,10 @@
       <c r="B16" t="s">
         <v>18</v>
       </c>
+      <c r="E16">
+        <f>(LEN(A16)-1)/3</f>
+        <v>36.333333333333336</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">

</xml_diff>